<commit_message>
Added readme and script to process antibiotic resistance data
</commit_message>
<xml_diff>
--- a/resistance_assay/20241114_Sink_Isolates_AR_22-11 and 22-5.xlsx
+++ b/resistance_assay/20241114_Sink_Isolates_AR_22-11 and 22-5.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tecan\Documents\Zhengqing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iridashyti/Documents/Duke_you_lab/sink_microbe_isolates/resistance_assay/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C38C87-D112-8741-AE36-1B72CE86655D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="21700" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="22-5" sheetId="2" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tecan</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -121,12 +122,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tecan</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -191,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -404,7 +405,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,13 +520,13 @@
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Tecan.At.Excel.Attenuation" xfId="6"/>
-    <cellStyle name="Tecan.At.Excel.AutoGain_0" xfId="7"/>
-    <cellStyle name="Tecan.At.Excel.Error" xfId="1"/>
-    <cellStyle name="Tecan.At.Excel.GFactorAndMeasurementBlank" xfId="5"/>
-    <cellStyle name="Tecan.At.Excel.GFactorBlank" xfId="3"/>
-    <cellStyle name="Tecan.At.Excel.GFactorReference" xfId="4"/>
-    <cellStyle name="Tecan.At.Excel.MeasurementBlank" xfId="2"/>
+    <cellStyle name="Tecan.At.Excel.Attenuation" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Tecan.At.Excel.AutoGain_0" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Tecan.At.Excel.Error" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Tecan.At.Excel.GFactorAndMeasurementBlank" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Tecan.At.Excel.GFactorBlank" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Tecan.At.Excel.GFactorReference" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Tecan.At.Excel.MeasurementBlank" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -802,16 +803,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -819,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -830,7 +831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -838,7 +839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -846,7 +847,7 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -854,7 +855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -862,7 +863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -870,7 +871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -878,12 +879,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -903,7 +904,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
@@ -923,7 +924,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -943,12 +944,12 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -956,7 +957,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -967,7 +968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -978,7 +979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -986,7 +987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -997,7 +998,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1005,7 +1006,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1013,12 +1014,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
@@ -1085,7 +1086,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
@@ -1120,7 +1121,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>41</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>42</v>
       </c>
@@ -1190,7 +1191,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>43</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
@@ -1260,7 +1261,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1275,16 +1276,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1292,7 +1293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1303,7 +1304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1311,7 +1312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1319,7 +1320,7 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1335,7 +1336,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1351,12 +1352,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -1376,7 +1377,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
@@ -1396,7 +1397,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1416,12 +1417,12 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1440,7 +1441,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1459,7 +1460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1470,7 +1471,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1486,12 +1487,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
@@ -1523,7 +1524,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
@@ -1558,7 +1559,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>41</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>42</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>43</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
@@ -1733,7 +1734,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1748,12 +1749,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>